<commit_message>
updated taxa,proteome list and code
</commit_message>
<xml_diff>
--- a/Book2.xlsx
+++ b/Book2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Phylogeny course\HWK\Get fasta seq\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8995E56-9A19-4C0A-8B04-3431B8E29805}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2264E11-2878-4C69-BC73-7A02DEC9E34B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10725" yWindow="1665" windowWidth="21600" windowHeight="11835" activeTab="2" xr2:uid="{8709ECF3-95D0-44C7-BA49-A85C71A50ED5}"/>
+    <workbookView xWindow="6825" yWindow="2160" windowWidth="21600" windowHeight="11835" activeTab="2" xr2:uid="{8709ECF3-95D0-44C7-BA49-A85C71A50ED5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2017" uniqueCount="829">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2023" uniqueCount="835">
   <si>
     <t>Species</t>
   </si>
@@ -2549,6 +2549,24 @@
   </si>
   <si>
     <t>1st tree</t>
+  </si>
+  <si>
+    <t>UP000001940</t>
+  </si>
+  <si>
+    <t>Caenorhabditis elegans (Strain: Bristol N2)</t>
+  </si>
+  <si>
+    <t>Mus musculus (Mouse)</t>
+  </si>
+  <si>
+    <t>UP000000589</t>
+  </si>
+  <si>
+    <t>Saccharomyces cerevisiae (strain ATCC 204508 / S288c) (Baker's yeast)</t>
+  </si>
+  <si>
+    <t>UP000002311</t>
   </si>
 </sst>
 </file>
@@ -7223,8 +7241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C364D0B-1F64-4547-A3B5-1F9C415458DB}">
   <dimension ref="A7:I160"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7236,203 +7254,234 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>2769</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>479</v>
+        <v>10090</v>
+      </c>
+      <c r="B8" t="s">
+        <v>832</v>
       </c>
       <c r="C8" t="s">
-        <v>478</v>
+        <v>831</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>280699</v>
+        <v>6239</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>481</v>
+        <v>829</v>
       </c>
       <c r="C9" t="s">
-        <v>480</v>
+        <v>830</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>130081</v>
+      <c r="A10">
+        <v>559292</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>473</v>
+        <v>834</v>
       </c>
       <c r="C10" t="s">
-        <v>472</v>
+        <v>833</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>3055</v>
+      <c r="A11" s="2">
+        <v>2769</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>469</v>
+        <v>479</v>
       </c>
       <c r="C11" t="s">
-        <v>468</v>
+        <v>478</v>
       </c>
       <c r="E11" t="s">
         <v>459</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>436017</v>
+      <c r="A12" s="2">
+        <v>280699</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>465</v>
+        <v>481</v>
       </c>
       <c r="C12" t="s">
-        <v>464</v>
+        <v>480</v>
       </c>
       <c r="E12" t="s">
         <v>459</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="2">
+        <v>130081</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="C13" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>3055</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="C14" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>436017</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="C15" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>69332</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C16" t="s">
         <v>454</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>1480154</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>451</v>
-      </c>
-      <c r="C14" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>3218</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>449</v>
-      </c>
-      <c r="C15" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>88036</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>446</v>
-      </c>
-      <c r="C16" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>13333</v>
+        <v>1480154</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C17" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
+        <v>3218</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="C18" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>88036</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="C19" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>13333</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="C20" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
         <v>39947</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C21" t="s">
         <v>386</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>4686</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>441</v>
-      </c>
-      <c r="C19" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
-        <v>3469</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>439</v>
-      </c>
-      <c r="C20" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>3702</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="C21" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>3694</v>
+        <v>4686</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>435</v>
+        <v>441</v>
       </c>
       <c r="C22" t="s">
-        <v>434</v>
+        <v>440</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>4081</v>
+      <c r="A23" s="4">
+        <v>3469</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>433</v>
+        <v>439</v>
       </c>
       <c r="C23" t="s">
-        <v>393</v>
+        <v>438</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>79200</v>
+        <v>3702</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>827</v>
+        <v>437</v>
       </c>
       <c r="C24" t="s">
-        <v>826</v>
+        <v>436</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>3694</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="C25" t="s">
+        <v>434</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>4081</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="C26" t="s">
+        <v>393</v>
+      </c>
       <c r="G26">
         <v>53036</v>
       </c>
       <c r="I26" t="s">
         <v>447</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>79200</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>827</v>
+      </c>
+      <c r="C27" t="s">
+        <v>826</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -8268,33 +8317,37 @@
     <hyperlink ref="H155" r:id="rId73" display="https://www.ebi.ac.uk/interpro/taxonomy/uniprot/156128/" xr:uid="{7FEE97E2-C37E-43E3-9AE6-C78AE41FCB93}"/>
     <hyperlink ref="H159" r:id="rId74" display="https://www.ebi.ac.uk/interpro/taxonomy/uniprot/195969/" xr:uid="{86C04AFE-EB74-4F99-A099-F3C42BFB91B4}"/>
     <hyperlink ref="H160" r:id="rId75" display="https://www.ebi.ac.uk/interpro/taxonomy/uniprot/2608996/" xr:uid="{4BEB16BF-6C3C-43BE-9403-D8D5D9774BC0}"/>
-    <hyperlink ref="A23" r:id="rId76" display="https://www.uniprot.org/taxonomy/4081" xr:uid="{B6740D01-9E9B-4240-B0CE-CD5EE06BF8BB}"/>
-    <hyperlink ref="B21" r:id="rId77" display="https://www.uniprot.org/proteomes/UP000006548" xr:uid="{9DB7C33A-861A-4060-9783-D712FEABBB61}"/>
-    <hyperlink ref="B22" r:id="rId78" display="https://www.uniprot.org/proteomes/UP000006729" xr:uid="{5C063B98-15DE-4394-B1F0-1434760A0DB0}"/>
-    <hyperlink ref="B23" r:id="rId79" display="https://www.uniprot.org/proteomes/UP000004994" xr:uid="{41F06C1A-5F3B-4363-9C00-B71C7A453849}"/>
-    <hyperlink ref="B24" r:id="rId80" display="https://www.uniprot.org/proteomes/UP000077755" xr:uid="{8070D789-15EC-4627-B998-D3C660753107}"/>
-    <hyperlink ref="A20" r:id="rId81" display="http://www.uniprot.org/taxonomy/3469" xr:uid="{BE89816C-A9A9-4DA5-B0F6-CFDA2B7FF3F2}"/>
-    <hyperlink ref="B20" r:id="rId82" display="https://www.uniprot.org/proteomes/UP000316621" xr:uid="{1E87DF53-C8DA-4CD5-834C-8A990C154BBC}"/>
-    <hyperlink ref="A18" r:id="rId83" display="https://www.uniprot.org/taxonomy/39947" xr:uid="{CA0FDD29-9B70-4B6B-9961-1E58AC65F1E4}"/>
-    <hyperlink ref="B18" r:id="rId84" display="https://www.uniprot.org/proteomes/UP000059680" xr:uid="{2BE31E17-425E-4423-A801-327973279EAA}"/>
-    <hyperlink ref="B19" r:id="rId85" display="https://www.uniprot.org/proteomes/UP000243459" xr:uid="{AB844436-9E14-4BE7-94AF-A2E74ECA9D7A}"/>
-    <hyperlink ref="A14" r:id="rId86" display="https://www.uniprot.org/taxonomy/1480154" xr:uid="{14B1A410-78D9-4ABD-A7A8-09DC021F61C9}"/>
-    <hyperlink ref="A15" r:id="rId87" display="https://www.uniprot.org/taxonomy/3218" xr:uid="{EFB3151B-42BB-415E-9ED6-D89059000B90}"/>
-    <hyperlink ref="A16" r:id="rId88" display="https://www.uniprot.org/taxonomy/88036" xr:uid="{5AAA35AF-B515-418D-98EB-5BF97A49CBDC}"/>
-    <hyperlink ref="A17" r:id="rId89" display="https://www.uniprot.org/taxonomy/13333" xr:uid="{8B8870FB-C58A-4BEC-B107-3F188E67A0D3}"/>
-    <hyperlink ref="B13" r:id="rId90" display="https://www.uniprot.org/proteomes/UP000265515" xr:uid="{44A5F225-E6C3-4424-9E1D-81415D53B8BF}"/>
-    <hyperlink ref="B17" r:id="rId91" display="https://www.uniprot.org/proteomes/UP000017836" xr:uid="{A7429F89-88DA-4269-93DD-B60AB81D1CDB}"/>
-    <hyperlink ref="B14" r:id="rId92" display="https://www.uniprot.org/proteomes/UP000077202" xr:uid="{2F594730-397B-4595-831F-50F403802EBB}"/>
-    <hyperlink ref="B15" r:id="rId93" display="https://www.uniprot.org/proteomes/UP000006727" xr:uid="{8DA5A567-EC24-46E9-9D8C-5FD98465C2C1}"/>
-    <hyperlink ref="B16" r:id="rId94" display="https://www.uniprot.org/proteomes/UP000001514" xr:uid="{BA5680CC-683D-4DD0-875A-911E56054154}"/>
-    <hyperlink ref="B11" r:id="rId95" display="https://www.uniprot.org/proteomes/UP000006906" xr:uid="{93D02222-8B39-4870-B085-30208A659F8C}"/>
-    <hyperlink ref="B12" r:id="rId96" display="https://www.uniprot.org/proteomes/UP000001568" xr:uid="{43221E9F-2307-45B2-8EE6-041F0FADFCA9}"/>
-    <hyperlink ref="A9" r:id="rId97" display="https://www.uniprot.org/taxonomy/280699" xr:uid="{146E4767-BA5D-4A8B-A9AF-A51E1FAC542C}"/>
-    <hyperlink ref="B9" r:id="rId98" display="https://www.uniprot.org/proteomes/UP000007014" xr:uid="{EDCAA847-F7FC-4A9A-8F1A-DCD21F16FCBD}"/>
-    <hyperlink ref="A8" r:id="rId99" display="https://www.uniprot.org/taxonomy/2769" xr:uid="{657D6934-AA45-48D1-A253-03B74199FF5A}"/>
-    <hyperlink ref="B8" r:id="rId100" display="https://www.uniprot.org/proteomes/UP000012073" xr:uid="{B8932B1E-69C7-413A-A4EA-881696949EE1}"/>
-    <hyperlink ref="A10" r:id="rId101" display="https://www.uniprot.org/taxonomy/130081" xr:uid="{2923C173-BBE8-4271-BD80-588A701B4E90}"/>
-    <hyperlink ref="B10" r:id="rId102" display="https://www.uniprot.org/proteomes/UP000030680" xr:uid="{B167E85C-1D8A-4152-9B3F-28BFEB62C7E7}"/>
+    <hyperlink ref="A26" r:id="rId76" display="https://www.uniprot.org/taxonomy/4081" xr:uid="{B6740D01-9E9B-4240-B0CE-CD5EE06BF8BB}"/>
+    <hyperlink ref="B24" r:id="rId77" display="https://www.uniprot.org/proteomes/UP000006548" xr:uid="{9DB7C33A-861A-4060-9783-D712FEABBB61}"/>
+    <hyperlink ref="B25" r:id="rId78" display="https://www.uniprot.org/proteomes/UP000006729" xr:uid="{5C063B98-15DE-4394-B1F0-1434760A0DB0}"/>
+    <hyperlink ref="B26" r:id="rId79" display="https://www.uniprot.org/proteomes/UP000004994" xr:uid="{41F06C1A-5F3B-4363-9C00-B71C7A453849}"/>
+    <hyperlink ref="B27" r:id="rId80" display="https://www.uniprot.org/proteomes/UP000077755" xr:uid="{8070D789-15EC-4627-B998-D3C660753107}"/>
+    <hyperlink ref="A23" r:id="rId81" display="http://www.uniprot.org/taxonomy/3469" xr:uid="{BE89816C-A9A9-4DA5-B0F6-CFDA2B7FF3F2}"/>
+    <hyperlink ref="B23" r:id="rId82" display="https://www.uniprot.org/proteomes/UP000316621" xr:uid="{1E87DF53-C8DA-4CD5-834C-8A990C154BBC}"/>
+    <hyperlink ref="A21" r:id="rId83" display="https://www.uniprot.org/taxonomy/39947" xr:uid="{CA0FDD29-9B70-4B6B-9961-1E58AC65F1E4}"/>
+    <hyperlink ref="B21" r:id="rId84" display="https://www.uniprot.org/proteomes/UP000059680" xr:uid="{2BE31E17-425E-4423-A801-327973279EAA}"/>
+    <hyperlink ref="B22" r:id="rId85" display="https://www.uniprot.org/proteomes/UP000243459" xr:uid="{AB844436-9E14-4BE7-94AF-A2E74ECA9D7A}"/>
+    <hyperlink ref="A17" r:id="rId86" display="https://www.uniprot.org/taxonomy/1480154" xr:uid="{14B1A410-78D9-4ABD-A7A8-09DC021F61C9}"/>
+    <hyperlink ref="A18" r:id="rId87" display="https://www.uniprot.org/taxonomy/3218" xr:uid="{EFB3151B-42BB-415E-9ED6-D89059000B90}"/>
+    <hyperlink ref="A19" r:id="rId88" display="https://www.uniprot.org/taxonomy/88036" xr:uid="{5AAA35AF-B515-418D-98EB-5BF97A49CBDC}"/>
+    <hyperlink ref="A20" r:id="rId89" display="https://www.uniprot.org/taxonomy/13333" xr:uid="{8B8870FB-C58A-4BEC-B107-3F188E67A0D3}"/>
+    <hyperlink ref="B16" r:id="rId90" display="https://www.uniprot.org/proteomes/UP000265515" xr:uid="{44A5F225-E6C3-4424-9E1D-81415D53B8BF}"/>
+    <hyperlink ref="B20" r:id="rId91" display="https://www.uniprot.org/proteomes/UP000017836" xr:uid="{A7429F89-88DA-4269-93DD-B60AB81D1CDB}"/>
+    <hyperlink ref="B17" r:id="rId92" display="https://www.uniprot.org/proteomes/UP000077202" xr:uid="{2F594730-397B-4595-831F-50F403802EBB}"/>
+    <hyperlink ref="B18" r:id="rId93" display="https://www.uniprot.org/proteomes/UP000006727" xr:uid="{8DA5A567-EC24-46E9-9D8C-5FD98465C2C1}"/>
+    <hyperlink ref="B19" r:id="rId94" display="https://www.uniprot.org/proteomes/UP000001514" xr:uid="{BA5680CC-683D-4DD0-875A-911E56054154}"/>
+    <hyperlink ref="B14" r:id="rId95" display="https://www.uniprot.org/proteomes/UP000006906" xr:uid="{93D02222-8B39-4870-B085-30208A659F8C}"/>
+    <hyperlink ref="B15" r:id="rId96" display="https://www.uniprot.org/proteomes/UP000001568" xr:uid="{43221E9F-2307-45B2-8EE6-041F0FADFCA9}"/>
+    <hyperlink ref="A12" r:id="rId97" display="https://www.uniprot.org/taxonomy/280699" xr:uid="{146E4767-BA5D-4A8B-A9AF-A51E1FAC542C}"/>
+    <hyperlink ref="B12" r:id="rId98" display="https://www.uniprot.org/proteomes/UP000007014" xr:uid="{EDCAA847-F7FC-4A9A-8F1A-DCD21F16FCBD}"/>
+    <hyperlink ref="A11" r:id="rId99" display="https://www.uniprot.org/taxonomy/2769" xr:uid="{657D6934-AA45-48D1-A253-03B74199FF5A}"/>
+    <hyperlink ref="B11" r:id="rId100" display="https://www.uniprot.org/proteomes/UP000012073" xr:uid="{B8932B1E-69C7-413A-A4EA-881696949EE1}"/>
+    <hyperlink ref="A13" r:id="rId101" display="https://www.uniprot.org/taxonomy/130081" xr:uid="{2923C173-BBE8-4271-BD80-588A701B4E90}"/>
+    <hyperlink ref="B13" r:id="rId102" display="https://www.uniprot.org/proteomes/UP000030680" xr:uid="{B167E85C-1D8A-4152-9B3F-28BFEB62C7E7}"/>
+    <hyperlink ref="B9" r:id="rId103" display="https://www.uniprot.org/proteomes/UP000001940" xr:uid="{DE360525-F3B7-400C-9709-4C35979931D9}"/>
+    <hyperlink ref="A9" r:id="rId104" display="https://www.uniprot.org/taxonomy/6239" xr:uid="{9B1828B8-F5B0-4C3A-9ED1-1C9906CEFAE7}"/>
+    <hyperlink ref="A8" r:id="rId105" display="https://www.uniprot.org/taxonomy/10090" xr:uid="{A905F2F6-966F-407D-A81C-E25E0679E1D4}"/>
+    <hyperlink ref="B10" r:id="rId106" display="https://www.uniprot.org/proteomes/UP000002311" xr:uid="{53490E3E-3C3A-47AF-93A7-E4F0AF12DC66}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
finally finished fasta list
</commit_message>
<xml_diff>
--- a/Book2.xlsx
+++ b/Book2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Phylogeny course\HWK\Get fasta seq\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Phylogeny course\HWK\BIOL525B_data_collection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2264E11-2878-4C69-BC73-7A02DEC9E34B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4CC5EA-1342-412E-91B7-E0A5EE2794AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6825" yWindow="2160" windowWidth="21600" windowHeight="11835" activeTab="2" xr2:uid="{8709ECF3-95D0-44C7-BA49-A85C71A50ED5}"/>
+    <workbookView xWindow="2715" yWindow="1920" windowWidth="21600" windowHeight="11835" activeTab="2" xr2:uid="{8709ECF3-95D0-44C7-BA49-A85C71A50ED5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2023" uniqueCount="835">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2073" uniqueCount="870">
   <si>
     <t>Species</t>
   </si>
@@ -2567,6 +2567,111 @@
   </si>
   <si>
     <t>UP000002311</t>
+  </si>
+  <si>
+    <t>Accessions containing 4T</t>
+  </si>
+  <si>
+    <t>A0A087SPH1</t>
+  </si>
+  <si>
+    <t>A0A1D2A8K8</t>
+  </si>
+  <si>
+    <t>green algae</t>
+  </si>
+  <si>
+    <t>A0A5J4Y697</t>
+  </si>
+  <si>
+    <t>A0A7S0CWI4</t>
+  </si>
+  <si>
+    <t>C1E5C4</t>
+  </si>
+  <si>
+    <t>C1N342</t>
+  </si>
+  <si>
+    <t>I0YIL4</t>
+  </si>
+  <si>
+    <t>A0A0G4GBC1</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>A0A1Q9CYF0</t>
+  </si>
+  <si>
+    <t>A0A7J6L3D7</t>
+  </si>
+  <si>
+    <t>A0A7J6L790</t>
+  </si>
+  <si>
+    <t>!!</t>
+  </si>
+  <si>
+    <t>A0A7J6MP59</t>
+  </si>
+  <si>
+    <t>A0A7J6N207</t>
+  </si>
+  <si>
+    <t>http://www.ebi.ac.uk/interpro/entry/InterPro/IPR008974/protein/UniProt/taxonomy/uniprot/2698737/?page_size=100&amp;cursor=a0a7j6nfa6#table</t>
+  </si>
+  <si>
+    <t>discoba</t>
+  </si>
+  <si>
+    <t>nothing</t>
+  </si>
+  <si>
+    <t>metamonada</t>
+  </si>
+  <si>
+    <t>no result</t>
+  </si>
+  <si>
+    <t>mala</t>
+  </si>
+  <si>
+    <t>hemimastigophora</t>
+  </si>
+  <si>
+    <t>crums</t>
+  </si>
+  <si>
+    <t>A0A151ZFB2</t>
+  </si>
+  <si>
+    <t>amoeba</t>
+  </si>
+  <si>
+    <t>F0ZKJ5</t>
+  </si>
+  <si>
+    <t>F4PU02</t>
+  </si>
+  <si>
+    <t>F4Q5N9</t>
+  </si>
+  <si>
+    <t>Q555F9</t>
+  </si>
+  <si>
+    <t>B0W2A4</t>
+  </si>
+  <si>
+    <t>metazoa</t>
+  </si>
+  <si>
+    <t>https://metazoa.ensembl.org/Branchiostoma_lanceolatum/Transcript/Sequence_Protein?db=core;g=BL10991;r=Sc0000022:1193660-1198171;t=BL10991_evm1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">these two convergent </t>
   </si>
 </sst>
 </file>
@@ -7239,10 +7344,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C364D0B-1F64-4547-A3B5-1F9C415458DB}">
-  <dimension ref="A7:I160"/>
+  <dimension ref="A7:J160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:B27"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="K62" sqref="K62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7482,6 +7587,215 @@
       </c>
       <c r="C27" t="s">
         <v>826</v>
+      </c>
+    </row>
+    <row r="34" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H34" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="35" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H35" s="2" t="s">
+        <v>836</v>
+      </c>
+      <c r="I35" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="36" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H36" s="2" t="s">
+        <v>837</v>
+      </c>
+      <c r="I36" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="37" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H37" s="2" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="38" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H38" s="2" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="39" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H39" s="2" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="40" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H40" s="2" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="41" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H41" s="2" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="42" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H42" s="2" t="s">
+        <v>844</v>
+      </c>
+      <c r="I42" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="43" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H43" s="2" t="s">
+        <v>846</v>
+      </c>
+      <c r="I43" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="44" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H44" s="2" t="s">
+        <v>847</v>
+      </c>
+      <c r="I44" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="45" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H45" s="2" t="s">
+        <v>848</v>
+      </c>
+      <c r="I45" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="46" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H46" s="2" t="s">
+        <v>850</v>
+      </c>
+      <c r="I46" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="47" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H47" s="2" t="s">
+        <v>851</v>
+      </c>
+      <c r="I47" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="49" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H49" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="51" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H51" t="s">
+        <v>853</v>
+      </c>
+      <c r="I51" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="52" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H52" t="s">
+        <v>855</v>
+      </c>
+      <c r="I52" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="53" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H53" t="s">
+        <v>857</v>
+      </c>
+      <c r="I53" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="54" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H54" t="s">
+        <v>858</v>
+      </c>
+      <c r="I54" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="55" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H55" t="s">
+        <v>859</v>
+      </c>
+      <c r="I55" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="56" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H56" s="2" t="s">
+        <v>860</v>
+      </c>
+      <c r="I56" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="57" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H57" s="2" t="s">
+        <v>862</v>
+      </c>
+      <c r="I57" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="58" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H58" s="2" t="s">
+        <v>863</v>
+      </c>
+      <c r="I58" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="59" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H59" s="2" t="s">
+        <v>864</v>
+      </c>
+      <c r="I59" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="60" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H60" s="2" t="s">
+        <v>865</v>
+      </c>
+      <c r="I60" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="62" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H62" t="s">
+        <v>866</v>
+      </c>
+      <c r="I62" t="s">
+        <v>867</v>
+      </c>
+      <c r="J62" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="63" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H63" t="s">
+        <v>868</v>
+      </c>
+      <c r="I63" t="s">
+        <v>867</v>
+      </c>
+      <c r="J63" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="66" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H66" s="2">
+        <v>13888</v>
+      </c>
+      <c r="I66" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -8348,6 +8662,25 @@
     <hyperlink ref="A9" r:id="rId104" display="https://www.uniprot.org/taxonomy/6239" xr:uid="{9B1828B8-F5B0-4C3A-9ED1-1C9906CEFAE7}"/>
     <hyperlink ref="A8" r:id="rId105" display="https://www.uniprot.org/taxonomy/10090" xr:uid="{A905F2F6-966F-407D-A81C-E25E0679E1D4}"/>
     <hyperlink ref="B10" r:id="rId106" display="https://www.uniprot.org/proteomes/UP000002311" xr:uid="{53490E3E-3C3A-47AF-93A7-E4F0AF12DC66}"/>
+    <hyperlink ref="H35" r:id="rId107" display="http://www.ebi.ac.uk/interpro/protein/unreviewed/A0A087SPH1/" xr:uid="{F28DF0FC-7A01-4CE5-B04F-808BD340F2FC}"/>
+    <hyperlink ref="H36" r:id="rId108" display="http://www.ebi.ac.uk/interpro/protein/unreviewed/A0A1D2A8K8/" xr:uid="{468BF7C7-BA5B-4DC1-BAD9-3E3AF2F3828A}"/>
+    <hyperlink ref="H66" r:id="rId109" display="https://phycocosm.jgi.doe.gov/cgi-bin/dispGeneModel?db=Cyapar1&amp;id=13888" xr:uid="{D7F83277-AB61-4DBB-991B-6925FE4320A4}"/>
+    <hyperlink ref="H37" r:id="rId110" display="http://www.ebi.ac.uk/interpro/protein/unreviewed/A0A5J4Y697/" xr:uid="{272F4BD7-26DA-4E0C-B234-6307AE40B495}"/>
+    <hyperlink ref="H38" r:id="rId111" display="http://www.ebi.ac.uk/interpro/protein/unreviewed/A0A7S0CWI4/" xr:uid="{401EE821-9F56-4F9F-BFD4-4196B0ADAAFB}"/>
+    <hyperlink ref="H39" r:id="rId112" display="http://www.ebi.ac.uk/interpro/protein/unreviewed/C1E5C4/" xr:uid="{80FCFB7C-4C98-446A-8EAE-D1A38AF7A7B8}"/>
+    <hyperlink ref="H40" r:id="rId113" display="http://www.ebi.ac.uk/interpro/protein/unreviewed/C1N342/" xr:uid="{A1214BE1-7013-4B7A-91CC-6D7EE6A4F596}"/>
+    <hyperlink ref="H41" r:id="rId114" display="http://www.ebi.ac.uk/interpro/protein/unreviewed/I0YIL4/" xr:uid="{2A8C0EE8-C0A7-4797-A68E-56C70F8FBCF1}"/>
+    <hyperlink ref="H42" r:id="rId115" display="http://www.ebi.ac.uk/interpro/protein/unreviewed/A0A0G4GBC1/" xr:uid="{9EC8648B-6A38-42A1-B757-E40860941E4A}"/>
+    <hyperlink ref="H43" r:id="rId116" display="http://www.ebi.ac.uk/interpro/protein/unreviewed/A0A1Q9CYF0/" xr:uid="{E40C7844-5049-41DD-AF41-FC803DC42FD7}"/>
+    <hyperlink ref="H44" r:id="rId117" display="http://www.ebi.ac.uk/interpro/protein/unreviewed/A0A7J6L3D7/" xr:uid="{55CA01CE-B6EE-4A67-B32B-1AD6BC6A39B7}"/>
+    <hyperlink ref="H45" r:id="rId118" display="http://www.ebi.ac.uk/interpro/protein/unreviewed/A0A7J6L790/" xr:uid="{581CE21F-0FAC-4A90-A6C8-DD0D121CF82B}"/>
+    <hyperlink ref="H46" r:id="rId119" display="http://www.ebi.ac.uk/interpro/protein/unreviewed/A0A7J6MP59/" xr:uid="{4EF6A1CB-331F-4461-A8E4-4E768E30E478}"/>
+    <hyperlink ref="H47" r:id="rId120" display="http://www.ebi.ac.uk/interpro/protein/unreviewed/A0A7J6N207/" xr:uid="{E86A603C-A087-45DA-ABA7-9C2CEA42076E}"/>
+    <hyperlink ref="H56" r:id="rId121" display="http://www.ebi.ac.uk/interpro/protein/unreviewed/A0A151ZFB2/" xr:uid="{F2E2281D-CACA-45CB-9661-746645F4759E}"/>
+    <hyperlink ref="H57" r:id="rId122" display="http://www.ebi.ac.uk/interpro/protein/unreviewed/F0ZKJ5/" xr:uid="{D40100C6-5BF2-4332-BBCA-D74F0CB28A36}"/>
+    <hyperlink ref="H58" r:id="rId123" display="http://www.ebi.ac.uk/interpro/protein/unreviewed/F4PU02/" xr:uid="{7CAB0C5E-249F-4C71-B9FF-D11DDF443874}"/>
+    <hyperlink ref="H59" r:id="rId124" display="http://www.ebi.ac.uk/interpro/protein/unreviewed/F4Q5N9/" xr:uid="{35A5A956-D6B2-40F4-B735-51CE708F25AC}"/>
+    <hyperlink ref="H60" r:id="rId125" display="http://www.ebi.ac.uk/interpro/protein/unreviewed/Q555F9/" xr:uid="{AB5BDC0A-1E14-437E-82ED-30F5EA187AD0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>